<commit_message>
recipes + feed + remove tv ta db
</commit_message>
<xml_diff>
--- a/scripts/work-pulse.xlsx
+++ b/scripts/work-pulse.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\PycharmProjects\potykion.github.io\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE52D31-A072-4239-9321-E6E76D8DA5F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41CCA54-92AB-4C06-9AE4-357D09640ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{2B2692C1-2028-4975-A8F7-C513352BE6D3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Пульс" sheetId="1" r:id="rId1"/>
+    <sheet name="Начисления" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>аг</t>
   </si>
@@ -51,6 +52,21 @@
   </si>
   <si>
     <t>отдых</t>
+  </si>
+  <si>
+    <t>привычка "закинуть чтото в блог"</t>
+  </si>
+  <si>
+    <t>чтение</t>
+  </si>
+  <si>
+    <t>Что</t>
+  </si>
+  <si>
+    <t>Категория</t>
+  </si>
+  <si>
+    <t>Сколько баллов</t>
   </si>
 </sst>
 </file>
@@ -162,7 +178,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$B$1</c:f>
+              <c:f>Пульс!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -182,7 +198,7 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$A$2:$A$19</c:f>
+              <c:f>Пульс!$A$2:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="18"/>
@@ -245,7 +261,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$B$2:$B$19</c:f>
+              <c:f>Пульс!$B$2:$B$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -271,6 +287,9 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
@@ -287,7 +306,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$C$1</c:f>
+              <c:f>Пульс!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -307,7 +326,7 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$A$2:$A$19</c:f>
+              <c:f>Пульс!$A$2:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="18"/>
@@ -370,7 +389,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$C$2:$C$19</c:f>
+              <c:f>Пульс!$C$2:$C$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -396,6 +415,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
@@ -412,7 +434,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$D$1</c:f>
+              <c:f>Пульс!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -432,7 +454,7 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$A$2:$A$19</c:f>
+              <c:f>Пульс!$A$2:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="18"/>
@@ -495,7 +517,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$D$2:$D$19</c:f>
+              <c:f>Пульс!$D$2:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -522,6 +544,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -537,7 +562,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$E$1</c:f>
+              <c:f>Пульс!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -557,7 +582,7 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$A$2:$A$19</c:f>
+              <c:f>Пульс!$A$2:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="18"/>
@@ -620,7 +645,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$E$2:$E$19</c:f>
+              <c:f>Пульс!$E$2:$E$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -646,7 +671,10 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1772,7 +1800,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1958,20 +1986,32 @@
         <v>5</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>45457</v>
       </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -2059,4 +2099,57 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9005C9BF-FB02-4574-8AA4-757E33886A08}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="28.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>